<commit_message>
before transition of UI to new datamodel
</commit_message>
<xml_diff>
--- a/data-raw/experiments.xlsx
+++ b/data-raw/experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michielnoback/git_projects/Rprojects/growthis/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36593A6-523A-C742-9A69-7B935BE595F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CC0C96-4A4A-3240-BE90-6D5C98FC481D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{A5DC4BFA-DFD9-0343-9B83-CB7F123E2B77}"/>
+    <workbookView xWindow="9300" yWindow="4020" windowWidth="24460" windowHeight="16940" xr2:uid="{A5DC4BFA-DFD9-0343-9B83-CB7F123E2B77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,33 +34,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>experiment_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>file_name</t>
   </si>
   <si>
-    <t>S_aureus_30jan2020.xlsx</t>
-  </si>
-  <si>
-    <t>aureus_2020_01_30</t>
-  </si>
-  <si>
-    <t>pneumoniae_2020_03_02</t>
-  </si>
-  <si>
-    <t>K_pneumoniae_2maart2020.xls</t>
-  </si>
-  <si>
-    <t>aureus_2021_11_12</t>
-  </si>
-  <si>
-    <t>S_aureus_stampersruw_12nov2021.xls</t>
-  </si>
-  <si>
-    <t>coli_2021_12_02</t>
+    <t>2-3-2020</t>
+  </si>
+  <si>
+    <t>30-1-2020</t>
+  </si>
+  <si>
+    <t>12-11-2021</t>
+  </si>
+  <si>
+    <t>2-12-2021</t>
+  </si>
+  <si>
+    <t>experiment_date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>K_pneumoniae_2maart2020_N.xls</t>
+  </si>
+  <si>
+    <t>S_aureus_30jan2020_N.xlsx</t>
+  </si>
+  <si>
+    <t>S_aureus_stampersruw_12nov2021_N.xls</t>
+  </si>
+  <si>
+    <t>E_coli_stampersruw_02dec2021_N.xlsx</t>
+  </si>
+  <si>
+    <t>S.aureus grown with red and white rose extracts</t>
+  </si>
+  <si>
+    <t>K.pneumoniae grown with red and white rose extracts</t>
+  </si>
+  <si>
+    <t>S.aureus grown with tulip stamen extracts</t>
+  </si>
+  <si>
+    <t>E.coli grown with red tulip stamen extracts</t>
   </si>
 </sst>
 </file>
@@ -104,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,57 +440,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1289D05-739D-9845-AEF7-9704272885C6}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
versions 0.1 with new datasets
</commit_message>
<xml_diff>
--- a/data-raw/experiments.xlsx
+++ b/data-raw/experiments.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michielnoback/git_projects/Rprojects/growthis/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CC0C96-4A4A-3240-BE90-6D5C98FC481D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070A80E6-44CE-2446-9C23-5ED21F73B4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="4020" windowWidth="24460" windowHeight="16940" xr2:uid="{A5DC4BFA-DFD9-0343-9B83-CB7F123E2B77}"/>
+    <workbookView xWindow="7300" yWindow="3720" windowWidth="24460" windowHeight="16940" xr2:uid="{A5DC4BFA-DFD9-0343-9B83-CB7F123E2B77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>file_name</t>
   </si>
@@ -69,16 +69,58 @@
     <t>E_coli_stampersruw_02dec2021_N.xlsx</t>
   </si>
   <si>
-    <t>S.aureus grown with red and white rose extracts</t>
-  </si>
-  <si>
-    <t>K.pneumoniae grown with red and white rose extracts</t>
-  </si>
-  <si>
-    <t>S.aureus grown with tulip stamen extracts</t>
-  </si>
-  <si>
-    <t>E.coli grown with red tulip stamen extracts</t>
+    <t>growth curves aeruginosa stampersruw 07mrt2022.xlsx</t>
+  </si>
+  <si>
+    <t>7-3-2022</t>
+  </si>
+  <si>
+    <t>P.aeruginosa with red tulip anther extracts</t>
+  </si>
+  <si>
+    <t>growth curves aeruginosa stampersruw 08feb2022.xlsx</t>
+  </si>
+  <si>
+    <t>8-2-2022</t>
+  </si>
+  <si>
+    <t>growth curves aureus stampersruw 31Jan2022.xlsx</t>
+  </si>
+  <si>
+    <t>31-1-2022</t>
+  </si>
+  <si>
+    <t>S.aureus with red and white rose extracts</t>
+  </si>
+  <si>
+    <t>K.pneumoniae with red and white rose extracts</t>
+  </si>
+  <si>
+    <t>S.aureus with tulip stamen extracts</t>
+  </si>
+  <si>
+    <t>E.coli with red tulip stamen extracts</t>
+  </si>
+  <si>
+    <t>S.aureus with red tulip anther extracts</t>
+  </si>
+  <si>
+    <t>growth curves ecoli stampersruw 02feb2022.xlsx</t>
+  </si>
+  <si>
+    <t>2-2-2022</t>
+  </si>
+  <si>
+    <t>E.coli with red tulip anther extracts</t>
+  </si>
+  <si>
+    <t>growth curves pneumoniae stampersruw 09eb2022.xlsx</t>
+  </si>
+  <si>
+    <t>9-2-2022</t>
+  </si>
+  <si>
+    <t>K.pneumoniae with red tulip anther extracts</t>
   </si>
 </sst>
 </file>
@@ -122,10 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,15 +483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1289D05-739D-9845-AEF7-9704272885C6}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
@@ -472,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -483,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -494,7 +537,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -505,7 +548,62 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new datasets and bugfix for install.packages
</commit_message>
<xml_diff>
--- a/data-raw/experiments.xlsx
+++ b/data-raw/experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michielnoback/git_projects/Rprojects/growthis/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michielnoback/git_projects/R_projects/growthis/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070A80E6-44CE-2446-9C23-5ED21F73B4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00E15F9-BCE0-9C47-9C18-87CCF36F9708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="3720" windowWidth="24460" windowHeight="16940" xr2:uid="{A5DC4BFA-DFD9-0343-9B83-CB7F123E2B77}"/>
+    <workbookView xWindow="9980" yWindow="7940" windowWidth="24460" windowHeight="14600" xr2:uid="{A5DC4BFA-DFD9-0343-9B83-CB7F123E2B77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>file_name</t>
   </si>
@@ -121,6 +121,78 @@
   </si>
   <si>
     <t>K.pneumoniae with red tulip anther extracts</t>
+  </si>
+  <si>
+    <t>growth curves kpneumoniae huas028 5april2022.xlsx</t>
+  </si>
+  <si>
+    <t>5-4-2022</t>
+  </si>
+  <si>
+    <t>growth curves paeruginosa huas028 7april2022.xlsx</t>
+  </si>
+  <si>
+    <t>7-4-2022</t>
+  </si>
+  <si>
+    <t>P.aeruginosa with red tulip stamen extract</t>
+  </si>
+  <si>
+    <t>K.pneumoniae with red tulip stamen extract</t>
+  </si>
+  <si>
+    <t>growth curves aureus huas033 28april2022.xls</t>
+  </si>
+  <si>
+    <t>28-4-2022</t>
+  </si>
+  <si>
+    <t>S.aureus with red tulip anther extract</t>
+  </si>
+  <si>
+    <t>S.aureus with Delphinidin-3-rutinoside</t>
+  </si>
+  <si>
+    <t>growth curves aureus stampersruw fractie 21mrt2022.xlsx</t>
+  </si>
+  <si>
+    <t>21-3-2022</t>
+  </si>
+  <si>
+    <t>growth curves aures huas028 22mrt2022.xlsx</t>
+  </si>
+  <si>
+    <t>22-3-2022</t>
+  </si>
+  <si>
+    <t>S.aureus with red tulip stamen extract</t>
+  </si>
+  <si>
+    <t>growth curves ecoli huas028 4april2022.xlsx</t>
+  </si>
+  <si>
+    <t>4-4-2022</t>
+  </si>
+  <si>
+    <t>E.coli with red tulip stamen extract</t>
+  </si>
+  <si>
+    <t>growth curves ecoli huas034 16mei2022.xlsx</t>
+  </si>
+  <si>
+    <t>16-5-2022</t>
+  </si>
+  <si>
+    <t>E.coli with Delphinidin-3-rutinoside</t>
+  </si>
+  <si>
+    <t>growth curves kpneumoniae huas034 31mei2022.xlsx</t>
+  </si>
+  <si>
+    <t>31-5-2022</t>
+  </si>
+  <si>
+    <t>K.pneumoniae with Delphinidin-3-rutinoside</t>
   </si>
 </sst>
 </file>
@@ -483,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1289D05-739D-9845-AEF7-9704272885C6}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,6 +678,94 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>